<commit_message>
validate 5 self softmax
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melody/Code/DistKernel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06884B5C-8B97-CA4D-A055-EF272A0E0E04}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C93872-5484-D140-B375-CAB933D50F97}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="580" windowWidth="25040" windowHeight="13940" xr2:uid="{9B35900A-692F-1247-989F-F2A6759FCF85}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="92">
   <si>
     <t>old_resnet50</t>
   </si>
@@ -293,6 +293,15 @@
   </si>
   <si>
     <t>combine+sge</t>
+  </si>
+  <si>
+    <t>combine+refine</t>
+  </si>
+  <si>
+    <t>combine17_resnet18_FP32</t>
+  </si>
+  <si>
+    <t>combiine4+skeleton(AC)</t>
   </si>
 </sst>
 </file>
@@ -1973,10 +1982,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA76B3B3-A97F-4D4E-9A0C-4CE57D2939CF}">
-  <dimension ref="A1:O44"/>
+  <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="97" workbookViewId="0">
-      <selection activeCell="J46" sqref="J46"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="97" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1984,7 +1993,7 @@
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
     <col min="5" max="7" width="14.33203125" customWidth="1"/>
     <col min="9" max="9" width="25.6640625" customWidth="1"/>
-    <col min="13" max="13" width="19.1640625" customWidth="1"/>
+    <col min="13" max="13" width="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
@@ -2577,7 +2586,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="8:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H33" t="s">
         <v>13</v>
       </c>
@@ -2592,7 +2601,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="8:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H34" t="s">
         <v>12</v>
       </c>
@@ -2609,7 +2618,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="8:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H35" t="s">
         <v>13</v>
       </c>
@@ -2626,7 +2635,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="8:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H36" t="s">
         <v>12</v>
       </c>
@@ -2643,7 +2652,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="8:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H37" t="s">
         <v>12</v>
       </c>
@@ -2660,7 +2669,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="8:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H39" t="s">
         <v>12</v>
       </c>
@@ -2677,7 +2686,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="8:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H41" t="s">
         <v>12</v>
       </c>
@@ -2691,7 +2700,7 @@
         <v>88.446700000000007</v>
       </c>
     </row>
-    <row r="42" spans="8:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H42" t="s">
         <v>11</v>
       </c>
@@ -2707,8 +2716,11 @@
       <c r="M42" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="43" spans="8:13" x14ac:dyDescent="0.2">
+      <c r="N42" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H43" t="s">
         <v>13</v>
       </c>
@@ -2725,7 +2737,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="8:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H44" t="s">
         <v>10</v>
       </c>
@@ -2737,6 +2749,23 @@
       </c>
       <c r="M44" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="H45" t="s">
+        <v>13</v>
+      </c>
+      <c r="I45" t="s">
+        <v>90</v>
+      </c>
+      <c r="J45">
+        <v>71.015600000000006</v>
+      </c>
+      <c r="K45">
+        <v>89.957899999999995</v>
+      </c>
+      <c r="M45" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>